<commit_message>
excel_data read properly, distance function
</commit_message>
<xml_diff>
--- a/Datasheet.xlsx
+++ b/Datasheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\AirlinePlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4E346F-CD43-4C53-8E9E-EC04CF5AA87B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{29914976-1F2C-4739-BA0A-CE1754920B6F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="96" windowWidth="16332" windowHeight="10836" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -659,7 +659,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1229,8 +1229,8 @@
   </sheetPr>
   <dimension ref="A1:AA113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1815,7 +1815,9 @@
       <c r="B10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
       <c r="D10" s="3">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Added some parameters in Excel, nothing important
</commit_message>
<xml_diff>
--- a/Datasheet.xlsx
+++ b/Datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hofma\AirlinePlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009E4C79-4547-4B00-BE42-3BAFBFA48483}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA46A3A-C992-4537-82F8-555A884292E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="96" windowWidth="16332" windowHeight="10836" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="125">
   <si>
     <t>Population data per city</t>
   </si>
@@ -479,6 +479,12 @@
   </si>
   <si>
     <t>k=0,0007196</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>MEDIAN</t>
   </si>
 </sst>
 </file>
@@ -11665,8 +11671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A7E274-3790-4FC3-A361-86E6193B7861}">
   <dimension ref="A1:Y268"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="E137" sqref="E137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -21575,6 +21581,13 @@
         <f>MAX(B116:U135)</f>
         <v>22.778875178571639</v>
       </c>
+      <c r="C137" t="s">
+        <v>123</v>
+      </c>
+      <c r="D137">
+        <f>AVERAGE(B116:U135)</f>
+        <v>7.1215554581247398</v>
+      </c>
     </row>
     <row r="138" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
@@ -21583,6 +21596,13 @@
       <c r="B138">
         <f>SMALL(B116:U135,COUNTIF($B$116:$U$135,0)+1)</f>
         <v>1.8054732661482831E-2</v>
+      </c>
+      <c r="C138" t="s">
+        <v>124</v>
+      </c>
+      <c r="D138">
+        <f>MEDIAN(B116:U135)</f>
+        <v>5.9757189954615555</v>
       </c>
     </row>
     <row r="140" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Hele dag aan excel_data, functions en OF voor P2 gewerkt
</commit_message>
<xml_diff>
--- a/Datasheet.xlsx
+++ b/Datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hofma\AirlinePlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA46A3A-C992-4537-82F8-555A884292E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E38612-12A3-4510-8049-0EBAD4A41A68}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="96" windowWidth="16332" windowHeight="10836" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
     <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -967,7 +967,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1994,8 +1994,8 @@
   </sheetPr>
   <dimension ref="A1:AA113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10076,7 +10076,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11671,8 +11671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A7E274-3790-4FC3-A361-86E6193B7861}">
   <dimension ref="A1:Y268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="E137" sqref="E137"/>
+    <sheetView tabSelected="1" topLeftCell="N216" workbookViewId="0">
+      <selection activeCell="Z241" sqref="Z241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -28795,16 +28795,20 @@
         <v>10</v>
       </c>
       <c r="V220">
-        <v>0</v>
+        <f t="shared" ref="V220:Y220" si="24">IF(V194&gt;0,ROUND(($K$2*((V142^$H$2)*(V168^$I$2))/(($L$2*V194)^$J$2)),0),0)</f>
+        <v>481</v>
       </c>
       <c r="W220">
-        <v>0</v>
+        <f t="shared" si="24"/>
+        <v>173</v>
       </c>
       <c r="X220">
-        <v>0</v>
+        <f t="shared" si="24"/>
+        <v>198</v>
       </c>
       <c r="Y220">
-        <v>0</v>
+        <f t="shared" si="24"/>
+        <v>226</v>
       </c>
     </row>
     <row r="221" spans="1:25" x14ac:dyDescent="0.25">
@@ -28892,16 +28896,20 @@
         <v>6</v>
       </c>
       <c r="V221">
-        <v>0</v>
+        <f t="shared" ref="V221:Y221" si="25">IF(V195&gt;0,ROUND(($K$2*((V143^$H$2)*(V169^$I$2))/(($L$2*V195)^$J$2)),0),0)</f>
+        <v>345</v>
       </c>
       <c r="W221">
-        <v>0</v>
+        <f t="shared" si="25"/>
+        <v>125</v>
       </c>
       <c r="X221">
-        <v>0</v>
+        <f t="shared" si="25"/>
+        <v>145</v>
       </c>
       <c r="Y221">
-        <v>0</v>
+        <f t="shared" si="25"/>
+        <v>164</v>
       </c>
     </row>
     <row r="222" spans="1:25" x14ac:dyDescent="0.25">
@@ -28989,16 +28997,20 @@
         <v>6</v>
       </c>
       <c r="V222">
-        <v>0</v>
+        <f t="shared" ref="V222:Y222" si="26">IF(V196&gt;0,ROUND(($K$2*((V144^$H$2)*(V170^$I$2))/(($L$2*V196)^$J$2)),0),0)</f>
+        <v>297</v>
       </c>
       <c r="W222">
-        <v>0</v>
+        <f t="shared" si="26"/>
+        <v>109</v>
       </c>
       <c r="X222">
-        <v>0</v>
+        <f t="shared" si="26"/>
+        <v>127</v>
       </c>
       <c r="Y222">
-        <v>0</v>
+        <f t="shared" si="26"/>
+        <v>141</v>
       </c>
     </row>
     <row r="223" spans="1:25" x14ac:dyDescent="0.25">
@@ -29086,16 +29098,20 @@
         <v>17</v>
       </c>
       <c r="V223">
-        <v>0</v>
+        <f t="shared" ref="V223:Y223" si="27">IF(V197&gt;0,ROUND(($K$2*((V145^$H$2)*(V171^$I$2))/(($L$2*V197)^$J$2)),0),0)</f>
+        <v>476</v>
       </c>
       <c r="W223">
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>170</v>
       </c>
       <c r="X223">
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>186</v>
       </c>
       <c r="Y223">
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>218</v>
       </c>
     </row>
     <row r="224" spans="1:25" x14ac:dyDescent="0.25">
@@ -29183,16 +29199,20 @@
         <v>9</v>
       </c>
       <c r="V224">
-        <v>0</v>
+        <f t="shared" ref="V224:Y224" si="28">IF(V198&gt;0,ROUND(($K$2*((V146^$H$2)*(V172^$I$2))/(($L$2*V198)^$J$2)),0),0)</f>
+        <v>313</v>
       </c>
       <c r="W224">
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>114</v>
       </c>
       <c r="X224">
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>128</v>
       </c>
       <c r="Y224">
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>146</v>
       </c>
     </row>
     <row r="225" spans="1:25" x14ac:dyDescent="0.25">
@@ -29280,16 +29300,20 @@
         <v>8</v>
       </c>
       <c r="V225">
-        <v>0</v>
+        <f t="shared" ref="V225:Y225" si="29">IF(V199&gt;0,ROUND(($K$2*((V147^$H$2)*(V173^$I$2))/(($L$2*V199)^$J$2)),0),0)</f>
+        <v>402</v>
       </c>
       <c r="W225">
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>149</v>
       </c>
       <c r="X225">
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>174</v>
       </c>
       <c r="Y225">
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>192</v>
       </c>
     </row>
     <row r="226" spans="1:25" x14ac:dyDescent="0.25">
@@ -29377,16 +29401,20 @@
         <v>9</v>
       </c>
       <c r="V226">
-        <v>0</v>
+        <f t="shared" ref="V226:Y226" si="30">IF(V200&gt;0,ROUND(($K$2*((V148^$H$2)*(V174^$I$2))/(($L$2*V200)^$J$2)),0),0)</f>
+        <v>404</v>
       </c>
       <c r="W226">
-        <v>0</v>
+        <f t="shared" si="30"/>
+        <v>152</v>
       </c>
       <c r="X226">
-        <v>0</v>
+        <f t="shared" si="30"/>
+        <v>175</v>
       </c>
       <c r="Y226">
-        <v>0</v>
+        <f t="shared" si="30"/>
+        <v>192</v>
       </c>
     </row>
     <row r="227" spans="1:25" x14ac:dyDescent="0.25">
@@ -29474,16 +29502,20 @@
         <v>8</v>
       </c>
       <c r="V227">
-        <v>0</v>
+        <f t="shared" ref="V227:Y227" si="31">IF(V201&gt;0,ROUND(($K$2*((V149^$H$2)*(V175^$I$2))/(($L$2*V201)^$J$2)),0),0)</f>
+        <v>463</v>
       </c>
       <c r="W227">
-        <v>0</v>
+        <f t="shared" si="31"/>
+        <v>160</v>
       </c>
       <c r="X227">
-        <v>0</v>
+        <f t="shared" si="31"/>
+        <v>181</v>
       </c>
       <c r="Y227">
-        <v>0</v>
+        <f t="shared" si="31"/>
+        <v>214</v>
       </c>
     </row>
     <row r="228" spans="1:25" x14ac:dyDescent="0.25">
@@ -29571,16 +29603,20 @@
         <v>5</v>
       </c>
       <c r="V228">
-        <v>0</v>
+        <f t="shared" ref="V228:Y228" si="32">IF(V202&gt;0,ROUND(($K$2*((V150^$H$2)*(V176^$I$2))/(($L$2*V202)^$J$2)),0),0)</f>
+        <v>357</v>
       </c>
       <c r="W228">
-        <v>0</v>
+        <f t="shared" si="32"/>
+        <v>135</v>
       </c>
       <c r="X228">
-        <v>0</v>
+        <f t="shared" si="32"/>
+        <v>164</v>
       </c>
       <c r="Y228">
-        <v>0</v>
+        <f t="shared" si="32"/>
+        <v>177</v>
       </c>
     </row>
     <row r="229" spans="1:25" x14ac:dyDescent="0.25">
@@ -29668,16 +29704,20 @@
         <v>10</v>
       </c>
       <c r="V229">
-        <v>0</v>
+        <f t="shared" ref="V229:Y229" si="33">IF(V203&gt;0,ROUND(($K$2*((V151^$H$2)*(V177^$I$2))/(($L$2*V203)^$J$2)),0),0)</f>
+        <v>177</v>
       </c>
       <c r="W229">
-        <v>0</v>
+        <f t="shared" si="33"/>
+        <v>62</v>
       </c>
       <c r="X229">
-        <v>0</v>
+        <f t="shared" si="33"/>
+        <v>66</v>
       </c>
       <c r="Y229">
-        <v>0</v>
+        <f t="shared" si="33"/>
+        <v>79</v>
       </c>
     </row>
     <row r="230" spans="1:25" x14ac:dyDescent="0.25">
@@ -29765,16 +29805,20 @@
         <v>11</v>
       </c>
       <c r="V230">
-        <v>0</v>
+        <f t="shared" ref="V230:Y230" si="34">IF(V204&gt;0,ROUND(($K$2*((V152^$H$2)*(V178^$I$2))/(($L$2*V204)^$J$2)),0),0)</f>
+        <v>646</v>
       </c>
       <c r="W230">
-        <v>0</v>
+        <f t="shared" si="34"/>
+        <v>241</v>
       </c>
       <c r="X230">
-        <v>0</v>
+        <f t="shared" si="34"/>
+        <v>285</v>
       </c>
       <c r="Y230">
-        <v>0</v>
+        <f t="shared" si="34"/>
+        <v>312</v>
       </c>
     </row>
     <row r="231" spans="1:25" x14ac:dyDescent="0.25">
@@ -29862,16 +29906,20 @@
         <v>3</v>
       </c>
       <c r="V231">
-        <v>0</v>
+        <f t="shared" ref="V231:Y231" si="35">IF(V205&gt;0,ROUND(($K$2*((V153^$H$2)*(V179^$I$2))/(($L$2*V205)^$J$2)),0),0)</f>
+        <v>253</v>
       </c>
       <c r="W231">
-        <v>0</v>
+        <f t="shared" si="35"/>
+        <v>97</v>
       </c>
       <c r="X231">
-        <v>0</v>
+        <f t="shared" si="35"/>
+        <v>121</v>
       </c>
       <c r="Y231">
-        <v>0</v>
+        <f t="shared" si="35"/>
+        <v>127</v>
       </c>
     </row>
     <row r="232" spans="1:25" x14ac:dyDescent="0.25">
@@ -29959,16 +30007,20 @@
         <v>3</v>
       </c>
       <c r="V232">
-        <v>0</v>
+        <f t="shared" ref="V232:Y232" si="36">IF(V206&gt;0,ROUND(($K$2*((V154^$H$2)*(V180^$I$2))/(($L$2*V206)^$J$2)),0),0)</f>
+        <v>208</v>
       </c>
       <c r="W232">
-        <v>0</v>
+        <f t="shared" si="36"/>
+        <v>79</v>
       </c>
       <c r="X232">
-        <v>0</v>
+        <f t="shared" si="36"/>
+        <v>96</v>
       </c>
       <c r="Y232">
-        <v>0</v>
+        <f t="shared" si="36"/>
+        <v>102</v>
       </c>
     </row>
     <row r="233" spans="1:25" x14ac:dyDescent="0.25">
@@ -29996,76 +30048,80 @@
         <v>31</v>
       </c>
       <c r="G233">
-        <f t="shared" ref="C233:U238" si="24">IF(G207&gt;0,ROUND(($G$2*((G155^$H$2)*(G181^$I$2))/(($L$2*G207)^$J$2)),0),0)</f>
+        <f t="shared" ref="C233:U238" si="37">IF(G207&gt;0,ROUND(($G$2*((G155^$H$2)*(G181^$I$2))/(($L$2*G207)^$J$2)),0),0)</f>
         <v>23</v>
       </c>
       <c r="H233">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>40</v>
       </c>
       <c r="I233">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>28</v>
       </c>
       <c r="J233">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>162</v>
       </c>
       <c r="K233">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>34</v>
       </c>
       <c r="L233">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>9</v>
       </c>
       <c r="M233">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>74</v>
       </c>
       <c r="N233">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>19</v>
       </c>
       <c r="O233">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>17</v>
       </c>
       <c r="P233">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="Q233">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>10</v>
       </c>
       <c r="R233">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>2</v>
       </c>
       <c r="S233">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>16</v>
       </c>
       <c r="T233">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>11</v>
       </c>
       <c r="U233">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="V233">
-        <v>0</v>
+        <f t="shared" ref="V233:Y233" si="38">IF(V207&gt;0,ROUND(($K$2*((V155^$H$2)*(V181^$I$2))/(($L$2*V207)^$J$2)),0),0)</f>
+        <v>265</v>
       </c>
       <c r="W233">
-        <v>0</v>
+        <f t="shared" si="38"/>
+        <v>93</v>
       </c>
       <c r="X233">
-        <v>0</v>
+        <f t="shared" si="38"/>
+        <v>107</v>
       </c>
       <c r="Y233">
-        <v>0</v>
+        <f t="shared" si="38"/>
+        <v>124</v>
       </c>
     </row>
     <row r="234" spans="1:25" x14ac:dyDescent="0.25">
@@ -30077,92 +30133,96 @@
         <v>54</v>
       </c>
       <c r="C234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>29</v>
       </c>
       <c r="D234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>21</v>
       </c>
       <c r="E234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>25</v>
       </c>
       <c r="F234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>20</v>
       </c>
       <c r="G234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>18</v>
       </c>
       <c r="H234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>45</v>
       </c>
       <c r="I234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>49</v>
       </c>
       <c r="J234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>17</v>
       </c>
       <c r="K234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>24</v>
       </c>
       <c r="L234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
       <c r="M234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>63</v>
       </c>
       <c r="N234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>18</v>
       </c>
       <c r="O234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>32</v>
       </c>
       <c r="P234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>10</v>
       </c>
       <c r="Q234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="R234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>8</v>
       </c>
       <c r="S234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
       <c r="T234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>21</v>
       </c>
       <c r="U234">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>3</v>
       </c>
       <c r="V234">
-        <v>0</v>
+        <f t="shared" ref="V234:Y234" si="39">IF(V208&gt;0,ROUND(($K$2*((V156^$H$2)*(V182^$I$2))/(($L$2*V208)^$J$2)),0),0)</f>
+        <v>170</v>
       </c>
       <c r="W234">
-        <v>0</v>
+        <f t="shared" si="39"/>
+        <v>66</v>
       </c>
       <c r="X234">
-        <v>0</v>
+        <f t="shared" si="39"/>
+        <v>79</v>
       </c>
       <c r="Y234">
-        <v>0</v>
+        <f t="shared" si="39"/>
+        <v>83</v>
       </c>
     </row>
     <row r="235" spans="1:25" x14ac:dyDescent="0.25">
@@ -30174,92 +30234,96 @@
         <v>13</v>
       </c>
       <c r="C235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>7</v>
       </c>
       <c r="D235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
       <c r="E235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
       <c r="F235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
       <c r="G235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
       <c r="H235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>9</v>
       </c>
       <c r="I235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>13</v>
       </c>
       <c r="J235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="K235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
       <c r="L235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>2</v>
       </c>
       <c r="M235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>11</v>
       </c>
       <c r="N235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>3</v>
       </c>
       <c r="O235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
       <c r="P235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>2</v>
       </c>
       <c r="Q235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>8</v>
       </c>
       <c r="R235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="S235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="T235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>8</v>
       </c>
       <c r="U235">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="V235">
-        <v>0</v>
+        <f t="shared" ref="V235:Y235" si="40">IF(V209&gt;0,ROUND(($K$2*((V157^$H$2)*(V183^$I$2))/(($L$2*V209)^$J$2)),0),0)</f>
+        <v>49</v>
       </c>
       <c r="W235">
-        <v>0</v>
+        <f t="shared" si="40"/>
+        <v>19</v>
       </c>
       <c r="X235">
-        <v>0</v>
+        <f t="shared" si="40"/>
+        <v>23</v>
       </c>
       <c r="Y235">
-        <v>0</v>
+        <f t="shared" si="40"/>
+        <v>24</v>
       </c>
     </row>
     <row r="236" spans="1:25" x14ac:dyDescent="0.25">
@@ -30271,92 +30335,96 @@
         <v>49</v>
       </c>
       <c r="C236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>19</v>
       </c>
       <c r="D236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>15</v>
       </c>
       <c r="E236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>11</v>
       </c>
       <c r="F236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>14</v>
       </c>
       <c r="G236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>9</v>
       </c>
       <c r="H236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>14</v>
       </c>
       <c r="I236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>12</v>
       </c>
       <c r="J236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>24</v>
       </c>
       <c r="K236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>16</v>
       </c>
       <c r="L236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
       <c r="M236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>26</v>
       </c>
       <c r="N236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>10</v>
       </c>
       <c r="O236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>8</v>
       </c>
       <c r="P236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>16</v>
       </c>
       <c r="Q236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
       <c r="R236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="S236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="T236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
       <c r="U236">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>3</v>
       </c>
       <c r="V236">
-        <v>0</v>
+        <f t="shared" ref="V236:Y236" si="41">IF(V210&gt;0,ROUND(($K$2*((V158^$H$2)*(V184^$I$2))/(($L$2*V210)^$J$2)),0),0)</f>
+        <v>271</v>
       </c>
       <c r="W236">
-        <v>0</v>
+        <f t="shared" si="41"/>
+        <v>90</v>
       </c>
       <c r="X236">
-        <v>0</v>
+        <f t="shared" si="41"/>
+        <v>103</v>
       </c>
       <c r="Y236">
-        <v>0</v>
+        <f t="shared" si="41"/>
+        <v>128</v>
       </c>
     </row>
     <row r="237" spans="1:25" x14ac:dyDescent="0.25">
@@ -30368,92 +30436,96 @@
         <v>63</v>
       </c>
       <c r="C237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>37</v>
       </c>
       <c r="D237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>22</v>
       </c>
       <c r="E237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>26</v>
       </c>
       <c r="F237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>36</v>
       </c>
       <c r="G237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>38</v>
       </c>
       <c r="H237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>46</v>
       </c>
       <c r="I237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>151</v>
       </c>
       <c r="J237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>19</v>
       </c>
       <c r="K237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>17</v>
       </c>
       <c r="L237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>9</v>
       </c>
       <c r="M237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>50</v>
       </c>
       <c r="N237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>12</v>
       </c>
       <c r="O237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>17</v>
       </c>
       <c r="P237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>11</v>
       </c>
       <c r="Q237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>21</v>
       </c>
       <c r="R237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>8</v>
       </c>
       <c r="S237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
       <c r="T237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="U237">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="V237">
-        <v>0</v>
+        <f t="shared" ref="V237:Y237" si="42">IF(V211&gt;0,ROUND(($K$2*((V159^$H$2)*(V185^$I$2))/(($L$2*V211)^$J$2)),0),0)</f>
+        <v>182</v>
       </c>
       <c r="W237">
-        <v>0</v>
+        <f t="shared" si="42"/>
+        <v>69</v>
       </c>
       <c r="X237">
-        <v>0</v>
+        <f t="shared" si="42"/>
+        <v>80</v>
       </c>
       <c r="Y237">
-        <v>0</v>
+        <f t="shared" si="42"/>
+        <v>87</v>
       </c>
     </row>
     <row r="238" spans="1:25" x14ac:dyDescent="0.25">
@@ -30465,92 +30537,96 @@
         <v>21</v>
       </c>
       <c r="C238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>10</v>
       </c>
       <c r="D238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
       <c r="E238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
       <c r="F238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>17</v>
       </c>
       <c r="G238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>9</v>
       </c>
       <c r="H238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>8</v>
       </c>
       <c r="I238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>9</v>
       </c>
       <c r="J238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>8</v>
       </c>
       <c r="K238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
       <c r="L238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>10</v>
       </c>
       <c r="M238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>11</v>
       </c>
       <c r="N238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>3</v>
       </c>
       <c r="O238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>3</v>
       </c>
       <c r="P238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="Q238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>3</v>
       </c>
       <c r="R238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="S238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>3</v>
       </c>
       <c r="T238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="U238">
-        <f t="shared" si="24"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="V238">
-        <v>0</v>
+        <f t="shared" ref="V238:Y238" si="43">IF(V212&gt;0,ROUND(($K$2*((V160^$H$2)*(V186^$I$2))/(($L$2*V212)^$J$2)),0),0)</f>
+        <v>128</v>
       </c>
       <c r="W238">
-        <v>0</v>
+        <f t="shared" si="43"/>
+        <v>44</v>
       </c>
       <c r="X238">
-        <v>0</v>
+        <f t="shared" si="43"/>
+        <v>46</v>
       </c>
       <c r="Y238">
-        <v>0</v>
+        <f t="shared" si="43"/>
+        <v>56</v>
       </c>
     </row>
     <row r="239" spans="1:25" x14ac:dyDescent="0.25">
@@ -30562,73 +30638,96 @@
         <v>1108</v>
       </c>
       <c r="C239">
-        <v>0</v>
+        <f t="shared" ref="C239:Y242" si="44">IF(C213&gt;0,ROUND(($K$2*((C161^$H$2)*(C187^$I$2))/(($L$2*C213)^$J$2)),0),0)</f>
+        <v>481</v>
       </c>
       <c r="D239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>345</v>
       </c>
       <c r="E239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>297</v>
       </c>
       <c r="F239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>476</v>
       </c>
       <c r="G239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>313</v>
       </c>
       <c r="H239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>402</v>
       </c>
       <c r="I239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>404</v>
       </c>
       <c r="J239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>463</v>
       </c>
       <c r="K239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>357</v>
       </c>
       <c r="L239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>177</v>
       </c>
       <c r="M239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>646</v>
       </c>
       <c r="N239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>253</v>
       </c>
       <c r="O239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>208</v>
       </c>
       <c r="P239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>265</v>
       </c>
       <c r="Q239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>170</v>
       </c>
       <c r="R239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>49</v>
       </c>
       <c r="S239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>271</v>
       </c>
       <c r="T239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>182</v>
       </c>
       <c r="U239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>128</v>
       </c>
       <c r="V239">
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="W239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>2055</v>
       </c>
       <c r="X239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>1439</v>
       </c>
       <c r="Y239">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>4477</v>
       </c>
     </row>
     <row r="240" spans="1:25" x14ac:dyDescent="0.25">
@@ -30636,77 +30735,100 @@
         <v>81</v>
       </c>
       <c r="B240">
-        <f t="shared" ref="B240:B242" si="25">IF(B214&gt;0,ROUND(($K$2*((B162^$H$2)*(B188^$I$2))/(($L$2*B214)^$J$2)),0),0)</f>
+        <f t="shared" ref="B240:Q242" si="45">IF(B214&gt;0,ROUND(($K$2*((B162^$H$2)*(B188^$I$2))/(($L$2*B214)^$J$2)),0),0)</f>
         <v>393</v>
       </c>
       <c r="C240">
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>173</v>
       </c>
       <c r="D240">
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>125</v>
       </c>
       <c r="E240">
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>109</v>
       </c>
       <c r="F240">
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>170</v>
       </c>
       <c r="G240">
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>114</v>
       </c>
       <c r="H240">
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>149</v>
       </c>
       <c r="I240">
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>152</v>
       </c>
       <c r="J240">
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>160</v>
       </c>
       <c r="K240">
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>135</v>
       </c>
       <c r="L240">
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>62</v>
       </c>
       <c r="M240">
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>241</v>
       </c>
       <c r="N240">
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>97</v>
       </c>
       <c r="O240">
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>79</v>
       </c>
       <c r="P240">
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>93</v>
       </c>
       <c r="Q240">
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>66</v>
       </c>
       <c r="R240">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>19</v>
       </c>
       <c r="S240">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>90</v>
       </c>
       <c r="T240">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>69</v>
       </c>
       <c r="U240">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>44</v>
       </c>
       <c r="V240">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>2055</v>
       </c>
       <c r="W240">
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="X240">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>1429</v>
       </c>
       <c r="Y240">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>1797</v>
       </c>
     </row>
     <row r="241" spans="1:25" x14ac:dyDescent="0.25">
@@ -30714,77 +30836,100 @@
         <v>82</v>
       </c>
       <c r="B241">
-        <f t="shared" si="25"/>
+        <f t="shared" si="45"/>
         <v>448</v>
       </c>
       <c r="C241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>198</v>
       </c>
       <c r="D241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>145</v>
       </c>
       <c r="E241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>127</v>
       </c>
       <c r="F241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>186</v>
       </c>
       <c r="G241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>128</v>
       </c>
       <c r="H241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>174</v>
       </c>
       <c r="I241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>175</v>
       </c>
       <c r="J241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>181</v>
       </c>
       <c r="K241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>164</v>
       </c>
       <c r="L241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>66</v>
       </c>
       <c r="M241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>285</v>
       </c>
       <c r="N241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>121</v>
       </c>
       <c r="O241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>96</v>
       </c>
       <c r="P241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>107</v>
       </c>
       <c r="Q241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>79</v>
       </c>
       <c r="R241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>23</v>
       </c>
       <c r="S241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>103</v>
       </c>
       <c r="T241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>80</v>
       </c>
       <c r="U241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>46</v>
       </c>
       <c r="V241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>1439</v>
       </c>
       <c r="W241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>1429</v>
       </c>
       <c r="X241">
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="Y241">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>1158</v>
       </c>
     </row>
     <row r="242" spans="1:25" x14ac:dyDescent="0.25">
@@ -30792,76 +30937,99 @@
         <v>83</v>
       </c>
       <c r="B242">
-        <f t="shared" si="25"/>
+        <f t="shared" si="45"/>
         <v>519</v>
       </c>
       <c r="C242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>226</v>
       </c>
       <c r="D242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>164</v>
       </c>
       <c r="E242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>141</v>
       </c>
       <c r="F242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>218</v>
       </c>
       <c r="G242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>146</v>
       </c>
       <c r="H242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>192</v>
       </c>
       <c r="I242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>192</v>
       </c>
       <c r="J242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>214</v>
       </c>
       <c r="K242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>177</v>
       </c>
       <c r="L242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>79</v>
       </c>
       <c r="M242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>312</v>
       </c>
       <c r="N242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>127</v>
       </c>
       <c r="O242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>102</v>
       </c>
       <c r="P242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>124</v>
       </c>
       <c r="Q242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>83</v>
       </c>
       <c r="R242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>24</v>
       </c>
       <c r="S242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>128</v>
       </c>
       <c r="T242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>87</v>
       </c>
       <c r="U242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>56</v>
       </c>
       <c r="V242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>4477</v>
       </c>
       <c r="W242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>1797</v>
       </c>
       <c r="X242">
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>1158</v>
       </c>
       <c r="Y242">
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -30951,79 +31119,79 @@
         <v>0</v>
       </c>
       <c r="C245" s="16">
-        <f t="shared" ref="C245:U245" si="26">C219-C50</f>
+        <f t="shared" ref="C245:U245" si="46">C219-C50</f>
         <v>-108</v>
       </c>
       <c r="D245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>-63</v>
       </c>
       <c r="E245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>-15</v>
       </c>
       <c r="F245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>-22</v>
       </c>
       <c r="G245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>-13</v>
       </c>
       <c r="H245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>-13</v>
       </c>
       <c r="I245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>-31</v>
       </c>
       <c r="J245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>19</v>
       </c>
       <c r="K245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>6</v>
       </c>
       <c r="L245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>9</v>
       </c>
       <c r="M245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>-23</v>
       </c>
       <c r="N245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="O245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>-5</v>
       </c>
       <c r="P245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>-19</v>
       </c>
       <c r="Q245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>-15</v>
       </c>
       <c r="R245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>-7</v>
       </c>
       <c r="S245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>3</v>
       </c>
       <c r="T245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>-4</v>
       </c>
       <c r="U245" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>9</v>
       </c>
     </row>
@@ -31032,83 +31200,83 @@
         <v>58</v>
       </c>
       <c r="B246" s="16">
-        <f t="shared" ref="B246:U246" si="27">B220-B51</f>
+        <f t="shared" ref="B246:U246" si="47">B220-B51</f>
         <v>-108</v>
       </c>
       <c r="C246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="D246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>-33</v>
       </c>
       <c r="E246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>-43</v>
       </c>
       <c r="F246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>-16</v>
       </c>
       <c r="G246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>-16</v>
       </c>
       <c r="H246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>-24</v>
       </c>
       <c r="I246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>-36</v>
       </c>
       <c r="J246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>-1</v>
       </c>
       <c r="K246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>1</v>
       </c>
       <c r="L246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>-14</v>
       </c>
       <c r="M246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>-37</v>
       </c>
       <c r="N246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>2</v>
       </c>
       <c r="O246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>-20</v>
       </c>
       <c r="P246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Q246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>-4</v>
       </c>
       <c r="R246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>-17</v>
       </c>
       <c r="S246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>-13</v>
       </c>
       <c r="T246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>-6</v>
       </c>
       <c r="U246" s="16">
-        <f t="shared" si="27"/>
+        <f t="shared" si="47"/>
         <v>-13</v>
       </c>
     </row>
@@ -31117,83 +31285,83 @@
         <v>60</v>
       </c>
       <c r="B247" s="16">
-        <f t="shared" ref="B247:U247" si="28">B221-B52</f>
+        <f t="shared" ref="B247:U247" si="48">B221-B52</f>
         <v>-63</v>
       </c>
       <c r="C247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>-33</v>
       </c>
       <c r="D247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="E247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>-15</v>
       </c>
       <c r="F247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>-23</v>
       </c>
       <c r="G247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>5</v>
       </c>
       <c r="H247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>-23</v>
       </c>
       <c r="I247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>-26</v>
       </c>
       <c r="J247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>3</v>
       </c>
       <c r="K247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>-7</v>
       </c>
       <c r="L247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>-8</v>
       </c>
       <c r="M247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>-13</v>
       </c>
       <c r="N247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>-5</v>
       </c>
       <c r="O247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>-3</v>
       </c>
       <c r="P247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>1</v>
       </c>
       <c r="Q247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>2</v>
       </c>
       <c r="R247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="S247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>12</v>
       </c>
       <c r="T247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>-13</v>
       </c>
       <c r="U247" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>-7</v>
       </c>
     </row>
@@ -31202,83 +31370,83 @@
         <v>62</v>
       </c>
       <c r="B248" s="16">
-        <f t="shared" ref="B248:U248" si="29">B222-B53</f>
+        <f t="shared" ref="B248:U248" si="49">B222-B53</f>
         <v>-15</v>
       </c>
       <c r="C248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>-43</v>
       </c>
       <c r="D248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>-15</v>
       </c>
       <c r="E248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="F248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>-9</v>
       </c>
       <c r="G248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>7</v>
       </c>
       <c r="H248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>-28</v>
       </c>
       <c r="I248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>2</v>
       </c>
       <c r="J248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>14</v>
       </c>
       <c r="K248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>-1</v>
       </c>
       <c r="L248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>-4</v>
       </c>
       <c r="M248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>-11</v>
       </c>
       <c r="N248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>-17</v>
       </c>
       <c r="O248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>-18</v>
       </c>
       <c r="P248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>-17</v>
       </c>
       <c r="Q248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>-11</v>
       </c>
       <c r="R248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>4</v>
       </c>
       <c r="S248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>-10</v>
       </c>
       <c r="T248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>-14</v>
       </c>
       <c r="U248" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>5</v>
       </c>
     </row>
@@ -31287,83 +31455,83 @@
         <v>64</v>
       </c>
       <c r="B249" s="16">
-        <f t="shared" ref="B249:U249" si="30">B223-B54</f>
+        <f t="shared" ref="B249:U249" si="50">B223-B54</f>
         <v>-22</v>
       </c>
       <c r="C249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>-16</v>
       </c>
       <c r="D249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>-23</v>
       </c>
       <c r="E249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>-9</v>
       </c>
       <c r="F249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="G249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>-37</v>
       </c>
       <c r="H249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>-14</v>
       </c>
       <c r="I249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>-11</v>
       </c>
       <c r="J249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>-17</v>
       </c>
       <c r="K249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>-2</v>
       </c>
       <c r="L249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>-35</v>
       </c>
       <c r="M249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>-24</v>
       </c>
       <c r="N249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>2</v>
       </c>
       <c r="O249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>-5</v>
       </c>
       <c r="P249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>-17</v>
       </c>
       <c r="Q249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>-12</v>
       </c>
       <c r="R249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>-15</v>
       </c>
       <c r="S249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>-3</v>
       </c>
       <c r="T249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>-15</v>
       </c>
       <c r="U249" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>-6</v>
       </c>
     </row>
@@ -31372,83 +31540,83 @@
         <v>65</v>
       </c>
       <c r="B250" s="16">
-        <f t="shared" ref="B250:U250" si="31">B224-B55</f>
+        <f t="shared" ref="B250:U250" si="51">B224-B55</f>
         <v>-13</v>
       </c>
       <c r="C250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>-16</v>
       </c>
       <c r="D250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>5</v>
       </c>
       <c r="E250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>7</v>
       </c>
       <c r="F250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>-37</v>
       </c>
       <c r="G250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="H250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>-6</v>
       </c>
       <c r="I250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>-40</v>
       </c>
       <c r="J250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>-6</v>
       </c>
       <c r="K250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>4</v>
       </c>
       <c r="L250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="M250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>-8</v>
       </c>
       <c r="N250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>8</v>
       </c>
       <c r="O250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>10</v>
       </c>
       <c r="P250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>6</v>
       </c>
       <c r="Q250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>-14</v>
       </c>
       <c r="R250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>-11</v>
       </c>
       <c r="S250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="T250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>-15</v>
       </c>
       <c r="U250" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>8</v>
       </c>
     </row>
@@ -31457,83 +31625,83 @@
         <v>66</v>
       </c>
       <c r="B251" s="16">
-        <f t="shared" ref="B251:U251" si="32">B225-B56</f>
+        <f t="shared" ref="B251:U251" si="52">B225-B56</f>
         <v>-13</v>
       </c>
       <c r="C251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>-24</v>
       </c>
       <c r="D251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>-23</v>
       </c>
       <c r="E251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>-28</v>
       </c>
       <c r="F251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>-14</v>
       </c>
       <c r="G251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>-6</v>
       </c>
       <c r="H251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="I251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>-15</v>
       </c>
       <c r="J251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>-8</v>
       </c>
       <c r="K251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>-1</v>
       </c>
       <c r="L251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>5</v>
       </c>
       <c r="M251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>-6</v>
       </c>
       <c r="N251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>3</v>
       </c>
       <c r="O251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>-3</v>
       </c>
       <c r="P251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>9</v>
       </c>
       <c r="Q251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>-5</v>
       </c>
       <c r="R251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="S251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>5</v>
       </c>
       <c r="T251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>-1</v>
       </c>
       <c r="U251" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="52"/>
         <v>-3</v>
       </c>
     </row>
@@ -31542,83 +31710,83 @@
         <v>67</v>
       </c>
       <c r="B252" s="16">
-        <f t="shared" ref="B252:U252" si="33">B226-B57</f>
+        <f t="shared" ref="B252:U252" si="53">B226-B57</f>
         <v>-31</v>
       </c>
       <c r="C252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>-36</v>
       </c>
       <c r="D252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>-26</v>
       </c>
       <c r="E252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>2</v>
       </c>
       <c r="F252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>-11</v>
       </c>
       <c r="G252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>-40</v>
       </c>
       <c r="H252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>-15</v>
       </c>
       <c r="I252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="J252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>12</v>
       </c>
       <c r="K252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>-22</v>
       </c>
       <c r="L252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>-13</v>
       </c>
       <c r="M252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>-24</v>
       </c>
       <c r="N252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>-3</v>
       </c>
       <c r="O252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>-2</v>
       </c>
       <c r="P252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>-6</v>
       </c>
       <c r="Q252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>1</v>
       </c>
       <c r="R252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>1</v>
       </c>
       <c r="S252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>-12</v>
       </c>
       <c r="T252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>-57</v>
       </c>
       <c r="U252" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>-9</v>
       </c>
     </row>
@@ -31627,83 +31795,83 @@
         <v>68</v>
       </c>
       <c r="B253" s="16">
-        <f t="shared" ref="B253:U253" si="34">B227-B58</f>
+        <f t="shared" ref="B253:U253" si="54">B227-B58</f>
         <v>19</v>
       </c>
       <c r="C253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>-1</v>
       </c>
       <c r="D253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>3</v>
       </c>
       <c r="E253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>14</v>
       </c>
       <c r="F253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>-17</v>
       </c>
       <c r="G253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>-6</v>
       </c>
       <c r="H253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>-8</v>
       </c>
       <c r="I253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>12</v>
       </c>
       <c r="J253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="K253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>17</v>
       </c>
       <c r="L253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>-4</v>
       </c>
       <c r="M253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>13</v>
       </c>
       <c r="N253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>-15</v>
       </c>
       <c r="O253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>-1</v>
       </c>
       <c r="P253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>-19</v>
       </c>
       <c r="Q253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>4</v>
       </c>
       <c r="R253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
       <c r="S253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>13</v>
       </c>
       <c r="T253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>-16</v>
       </c>
       <c r="U253" s="16">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>7</v>
       </c>
     </row>
@@ -31712,83 +31880,83 @@
         <v>69</v>
       </c>
       <c r="B254" s="16">
-        <f t="shared" ref="B254:U254" si="35">B228-B59</f>
+        <f t="shared" ref="B254:U254" si="55">B228-B59</f>
         <v>6</v>
       </c>
       <c r="C254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>1</v>
       </c>
       <c r="D254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>-7</v>
       </c>
       <c r="E254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>-1</v>
       </c>
       <c r="F254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>-2</v>
       </c>
       <c r="G254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>4</v>
       </c>
       <c r="H254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>-1</v>
       </c>
       <c r="I254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>-22</v>
       </c>
       <c r="J254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>17</v>
       </c>
       <c r="K254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="L254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>9</v>
       </c>
       <c r="M254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>-13</v>
       </c>
       <c r="N254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>-10</v>
       </c>
       <c r="O254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>8</v>
       </c>
       <c r="P254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>-5</v>
       </c>
       <c r="Q254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>8</v>
       </c>
       <c r="R254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>2</v>
       </c>
       <c r="S254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>1</v>
       </c>
       <c r="T254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>9</v>
       </c>
       <c r="U254" s="16">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>4</v>
       </c>
     </row>
@@ -31797,83 +31965,83 @@
         <v>70</v>
       </c>
       <c r="B255" s="16">
-        <f t="shared" ref="B255:U255" si="36">B229-B60</f>
+        <f t="shared" ref="B255:U255" si="56">B229-B60</f>
         <v>9</v>
       </c>
       <c r="C255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>-14</v>
       </c>
       <c r="D255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>-8</v>
       </c>
       <c r="E255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>-4</v>
       </c>
       <c r="F255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>-35</v>
       </c>
       <c r="G255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="H255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>5</v>
       </c>
       <c r="I255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>-13</v>
       </c>
       <c r="J255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>-4</v>
       </c>
       <c r="K255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>9</v>
       </c>
       <c r="L255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="M255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="N255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>-1</v>
       </c>
       <c r="O255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="P255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>-2</v>
       </c>
       <c r="Q255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>-13</v>
       </c>
       <c r="R255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>-13</v>
       </c>
       <c r="S255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>4</v>
       </c>
       <c r="T255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>-10</v>
       </c>
       <c r="U255" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>-16</v>
       </c>
     </row>
@@ -31882,83 +32050,83 @@
         <v>71</v>
       </c>
       <c r="B256" s="16">
-        <f t="shared" ref="B256:U256" si="37">B230-B61</f>
+        <f t="shared" ref="B256:U256" si="57">B230-B61</f>
         <v>-23</v>
       </c>
       <c r="C256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>-37</v>
       </c>
       <c r="D256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>-13</v>
       </c>
       <c r="E256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>-11</v>
       </c>
       <c r="F256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>-24</v>
       </c>
       <c r="G256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>-8</v>
       </c>
       <c r="H256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>-6</v>
       </c>
       <c r="I256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>-24</v>
       </c>
       <c r="J256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>13</v>
       </c>
       <c r="K256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>-13</v>
       </c>
       <c r="L256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="M256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="N256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>-17</v>
       </c>
       <c r="O256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>-16</v>
       </c>
       <c r="P256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>-5</v>
       </c>
       <c r="Q256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>-11</v>
       </c>
       <c r="R256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>-1</v>
       </c>
       <c r="S256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>-12</v>
       </c>
       <c r="T256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>-17</v>
       </c>
       <c r="U256" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>-1</v>
       </c>
     </row>
@@ -31967,83 +32135,83 @@
         <v>72</v>
       </c>
       <c r="B257" s="16">
-        <f t="shared" ref="B257:U257" si="38">B231-B62</f>
+        <f t="shared" ref="B257:U257" si="58">B231-B62</f>
         <v>0</v>
       </c>
       <c r="C257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>2</v>
       </c>
       <c r="D257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>-5</v>
       </c>
       <c r="E257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>-17</v>
       </c>
       <c r="F257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>2</v>
       </c>
       <c r="G257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>8</v>
       </c>
       <c r="H257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>3</v>
       </c>
       <c r="I257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>-3</v>
       </c>
       <c r="J257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>-15</v>
       </c>
       <c r="K257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>-10</v>
       </c>
       <c r="L257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>-1</v>
       </c>
       <c r="M257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>-17</v>
       </c>
       <c r="N257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="O257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>-3</v>
       </c>
       <c r="P257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>-16</v>
       </c>
       <c r="Q257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>-9</v>
       </c>
       <c r="R257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="S257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>9</v>
       </c>
       <c r="T257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>9</v>
       </c>
       <c r="U257" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="58"/>
         <v>2</v>
       </c>
     </row>
@@ -32052,83 +32220,83 @@
         <v>73</v>
       </c>
       <c r="B258" s="16">
-        <f t="shared" ref="B258:U258" si="39">B232-B63</f>
+        <f t="shared" ref="B258:U258" si="59">B232-B63</f>
         <v>-5</v>
       </c>
       <c r="C258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>-20</v>
       </c>
       <c r="D258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>-3</v>
       </c>
       <c r="E258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>-18</v>
       </c>
       <c r="F258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>-5</v>
       </c>
       <c r="G258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>10</v>
       </c>
       <c r="H258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>-3</v>
       </c>
       <c r="I258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>-2</v>
       </c>
       <c r="J258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>-1</v>
       </c>
       <c r="K258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>8</v>
       </c>
       <c r="L258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>6</v>
       </c>
       <c r="M258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>-16</v>
       </c>
       <c r="N258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>-3</v>
       </c>
       <c r="O258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="P258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>-15</v>
       </c>
       <c r="Q258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>2</v>
       </c>
       <c r="R258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="S258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>-13</v>
       </c>
       <c r="T258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>8</v>
       </c>
       <c r="U258" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>-9</v>
       </c>
     </row>
@@ -32137,83 +32305,83 @@
         <v>74</v>
       </c>
       <c r="B259" s="16">
-        <f t="shared" ref="B259:U259" si="40">B233-B64</f>
+        <f t="shared" ref="B259:U259" si="60">B233-B64</f>
         <v>-19</v>
       </c>
       <c r="C259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="D259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>1</v>
       </c>
       <c r="E259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>-17</v>
       </c>
       <c r="F259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>-17</v>
       </c>
       <c r="G259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>6</v>
       </c>
       <c r="H259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>9</v>
       </c>
       <c r="I259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>-6</v>
       </c>
       <c r="J259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>-19</v>
       </c>
       <c r="K259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>-5</v>
       </c>
       <c r="L259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>-2</v>
       </c>
       <c r="M259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>-5</v>
       </c>
       <c r="N259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>-16</v>
       </c>
       <c r="O259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>-15</v>
       </c>
       <c r="P259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="Q259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>-3</v>
       </c>
       <c r="R259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>1</v>
       </c>
       <c r="S259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="T259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>-13</v>
       </c>
       <c r="U259" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="60"/>
         <v>3</v>
       </c>
     </row>
@@ -32222,83 +32390,83 @@
         <v>75</v>
       </c>
       <c r="B260" s="16">
-        <f t="shared" ref="B260:U260" si="41">B234-B65</f>
+        <f t="shared" ref="B260:U260" si="61">B234-B65</f>
         <v>-15</v>
       </c>
       <c r="C260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>-4</v>
       </c>
       <c r="D260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>2</v>
       </c>
       <c r="E260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>-11</v>
       </c>
       <c r="F260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>-12</v>
       </c>
       <c r="G260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>-14</v>
       </c>
       <c r="H260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>-5</v>
       </c>
       <c r="I260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>1</v>
       </c>
       <c r="J260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>4</v>
       </c>
       <c r="K260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>8</v>
       </c>
       <c r="L260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>-13</v>
       </c>
       <c r="M260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>-11</v>
       </c>
       <c r="N260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>-9</v>
       </c>
       <c r="O260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>2</v>
       </c>
       <c r="P260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>-3</v>
       </c>
       <c r="Q260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="R260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>-15</v>
       </c>
       <c r="S260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>4</v>
       </c>
       <c r="T260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>-14</v>
       </c>
       <c r="U260" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="61"/>
         <v>-6</v>
       </c>
     </row>
@@ -32307,83 +32475,83 @@
         <v>76</v>
       </c>
       <c r="B261" s="16">
-        <f t="shared" ref="B261:U261" si="42">B235-B66</f>
+        <f t="shared" ref="B261:U261" si="62">B235-B66</f>
         <v>-7</v>
       </c>
       <c r="C261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>-17</v>
       </c>
       <c r="D261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="E261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>4</v>
       </c>
       <c r="F261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>-15</v>
       </c>
       <c r="G261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>-11</v>
       </c>
       <c r="H261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="I261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="J261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="K261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>2</v>
       </c>
       <c r="L261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>-13</v>
       </c>
       <c r="M261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>-1</v>
       </c>
       <c r="N261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="O261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="P261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="Q261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>-15</v>
       </c>
       <c r="R261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="S261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="T261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>-8</v>
       </c>
       <c r="U261" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="62"/>
         <v>-13</v>
       </c>
     </row>
@@ -32392,83 +32560,83 @@
         <v>77</v>
       </c>
       <c r="B262" s="16">
-        <f t="shared" ref="B262:U262" si="43">B236-B67</f>
+        <f t="shared" ref="B262:U262" si="63">B236-B67</f>
         <v>3</v>
       </c>
       <c r="C262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>-13</v>
       </c>
       <c r="D262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>12</v>
       </c>
       <c r="E262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>-10</v>
       </c>
       <c r="F262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>-3</v>
       </c>
       <c r="G262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="H262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>5</v>
       </c>
       <c r="I262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>-12</v>
       </c>
       <c r="J262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>13</v>
       </c>
       <c r="K262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>1</v>
       </c>
       <c r="L262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>4</v>
       </c>
       <c r="M262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>-12</v>
       </c>
       <c r="N262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>9</v>
       </c>
       <c r="O262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>-13</v>
       </c>
       <c r="P262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="Q262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>4</v>
       </c>
       <c r="R262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="S262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="T262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>-14</v>
       </c>
       <c r="U262" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="63"/>
         <v>-2</v>
       </c>
     </row>
@@ -32477,83 +32645,83 @@
         <v>78</v>
       </c>
       <c r="B263" s="16">
-        <f t="shared" ref="B263:U263" si="44">B237-B68</f>
+        <f t="shared" ref="B263:U263" si="64">B237-B68</f>
         <v>-4</v>
       </c>
       <c r="C263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>-6</v>
       </c>
       <c r="D263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>-13</v>
       </c>
       <c r="E263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>-14</v>
       </c>
       <c r="F263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>-15</v>
       </c>
       <c r="G263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>-15</v>
       </c>
       <c r="H263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>-1</v>
       </c>
       <c r="I263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>-57</v>
       </c>
       <c r="J263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>-16</v>
       </c>
       <c r="K263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>9</v>
       </c>
       <c r="L263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>-10</v>
       </c>
       <c r="M263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>-17</v>
       </c>
       <c r="N263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>9</v>
       </c>
       <c r="O263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>8</v>
       </c>
       <c r="P263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>-13</v>
       </c>
       <c r="Q263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>-14</v>
       </c>
       <c r="R263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>-8</v>
       </c>
       <c r="S263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>-14</v>
       </c>
       <c r="T263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="U263" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="64"/>
         <v>3</v>
       </c>
     </row>
@@ -32562,83 +32730,83 @@
         <v>79</v>
       </c>
       <c r="B264" s="16">
-        <f t="shared" ref="B264:U264" si="45">B238-B69</f>
+        <f t="shared" ref="B264:U264" si="65">B238-B69</f>
         <v>9</v>
       </c>
       <c r="C264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>-13</v>
       </c>
       <c r="D264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>-7</v>
       </c>
       <c r="E264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>5</v>
       </c>
       <c r="F264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>-6</v>
       </c>
       <c r="G264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>8</v>
       </c>
       <c r="H264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>-3</v>
       </c>
       <c r="I264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>-9</v>
       </c>
       <c r="J264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>7</v>
       </c>
       <c r="K264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>4</v>
       </c>
       <c r="L264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>-16</v>
       </c>
       <c r="M264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>-1</v>
       </c>
       <c r="N264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>2</v>
       </c>
       <c r="O264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>-9</v>
       </c>
       <c r="P264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>3</v>
       </c>
       <c r="Q264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>-6</v>
       </c>
       <c r="R264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>-13</v>
       </c>
       <c r="S264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>-2</v>
       </c>
       <c r="T264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>3</v>
       </c>
       <c r="U264" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Some validation done and testing of the code
</commit_message>
<xml_diff>
--- a/Datasheet.xlsx
+++ b/Datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hofma\AirlinePlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB10868-C297-4360-BBC2-E9CB7BCC5AC1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829FE955-705D-478A-848D-16BA63FB55DD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="96" windowWidth="16332" windowHeight="10836" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1995,7 +1995,7 @@
   <dimension ref="A1:AA113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10076,7 +10076,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>